<commit_message>
Fixed Bill bifurcation issue
</commit_message>
<xml_diff>
--- a/modules/purchase/uploads/file_sample/Sample_pur_bills_en.xlsx
+++ b/modules/purchase/uploads/file_sample/Sample_pur_bills_en.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Bill Id</t>
   </si>
@@ -31,6 +31,24 @@
   </si>
   <si>
     <t>Qty</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
   </si>
 </sst>
 </file>
@@ -375,7 +393,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -383,10 +401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15"/>
@@ -412,6 +430,36 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>